<commit_message>
sm5g sm5g-b axp15060 support
Change-Id: I0de692aabed6fa5172475dad947697e6f404b71e

Former-commit-id: 4e2ae8d154395d0c396879913d3f50b182738917
</commit_message>
<xml_diff>
--- a/SM5G/config.xlsx
+++ b/SM5G/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowHeight="18255" tabRatio="500" activeTab="1"/>
+    <workbookView windowWidth="28740" windowHeight="12795" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="pin" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="138">
   <si>
     <t>Pin number</t>
   </si>
@@ -118,6 +118,9 @@
     <t>PA15</t>
   </si>
   <si>
+    <t>PCIE_RRST_OUT</t>
+  </si>
+  <si>
     <t>PA2</t>
   </si>
   <si>
@@ -199,15 +202,18 @@
     <t>PB12</t>
   </si>
   <si>
+    <t>PCIE_RRST_IN</t>
+  </si>
+  <si>
+    <t>INPUT</t>
+  </si>
+  <si>
     <t>PB13</t>
   </si>
   <si>
     <t>AXP_IRQ</t>
   </si>
   <si>
-    <t>INPUT</t>
-  </si>
-  <si>
     <t>PB14</t>
   </si>
   <si>
@@ -325,7 +331,7 @@
     <t>VDD-3.3V-CLOCK</t>
   </si>
   <si>
-    <t>PMIC_ALDO2</t>
+    <t>PMIC_ALDO_2</t>
   </si>
   <si>
     <t>FUNCTION</t>
@@ -334,7 +340,7 @@
     <t>VDD-1.8V</t>
   </si>
   <si>
-    <t>PMIC_CHANNEL_6</t>
+    <t>PMIC_DCDC_6</t>
   </si>
   <si>
     <t>VDD-CORE</t>
@@ -352,13 +358,13 @@
     <t>DDR-VDDQ</t>
   </si>
   <si>
-    <t>PMIC_CHANNEL_5</t>
+    <t>PMIC_DCDC_5</t>
   </si>
   <si>
     <t>VDD-QLP-3.3V-0.8V</t>
   </si>
   <si>
-    <t>PMIC_CHANNEL_1234</t>
+    <t>PMIC_DCDC_1234</t>
   </si>
   <si>
     <t>ACK-P08</t>
@@ -394,7 +400,7 @@
     <t>VQPS-1.8V</t>
   </si>
   <si>
-    <t>PMIC_ALDO1</t>
+    <t>PMIC_ALDO_1</t>
   </si>
   <si>
     <t>SYS-RST-DEASSERT</t>
@@ -467,8 +473,16 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -482,24 +496,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -511,25 +519,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -543,9 +534,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -558,10 +548,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -573,8 +572,24 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -594,17 +609,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -637,19 +643,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -661,163 +823,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -832,40 +838,16 @@
     </border>
     <border>
       <left style="hair">
-        <color auto="true"/>
+        <color auto="1"/>
       </left>
       <right style="hair">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top style="hair">
-        <color auto="true"/>
+        <color auto="1"/>
       </top>
       <bottom style="hair">
-        <color auto="true"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -879,17 +861,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -935,6 +911,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -943,181 +934,193 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="left" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="left" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
-      <alignment horizontal="left" wrapText="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1366,7 +1369,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1390,9 +1393,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1416,7 +1419,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -1469,7 +1472,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1494,7 +1497,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -1508,56 +1511,56 @@
   <sheetPr/>
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="14.88" style="9" customWidth="true"/>
-    <col min="2" max="2" width="16.38" style="10" customWidth="true"/>
-    <col min="3" max="3" width="21.3733333333333" style="9" customWidth="true"/>
-    <col min="4" max="4" width="8.78666666666667" style="9" customWidth="true"/>
-    <col min="5" max="5" width="9.13333333333333" style="9" customWidth="true"/>
-    <col min="6" max="6" width="12.3666666666667" style="9" customWidth="true"/>
-    <col min="7" max="7" width="14.2133333333333" style="9" customWidth="true"/>
-    <col min="8" max="8" width="15.9466666666667" style="9" customWidth="true"/>
-    <col min="9" max="9" width="9.13333333333333" style="9" customWidth="true"/>
-    <col min="10" max="10" width="93.1266666666667" style="9" customWidth="true"/>
-    <col min="11" max="1022" width="9" style="9" customWidth="true"/>
-    <col min="1023" max="1023" width="11.52" style="9"/>
+    <col min="1" max="1" width="14.88" style="8" customWidth="1"/>
+    <col min="2" max="2" width="16.38" style="9" customWidth="1"/>
+    <col min="3" max="3" width="21.3733333333333" style="8" customWidth="1"/>
+    <col min="4" max="4" width="8.78666666666667" style="8" customWidth="1"/>
+    <col min="5" max="5" width="9.13333333333333" style="8" customWidth="1"/>
+    <col min="6" max="6" width="12.3666666666667" style="8" customWidth="1"/>
+    <col min="7" max="7" width="14.2133333333333" style="8" customWidth="1"/>
+    <col min="8" max="8" width="15.9466666666667" style="8" customWidth="1"/>
+    <col min="9" max="9" width="9.13333333333333" style="8" customWidth="1"/>
+    <col min="10" max="10" width="93.1266666666667" style="8" customWidth="1"/>
+    <col min="11" max="1022" width="9" style="8" customWidth="1"/>
+    <col min="1023" max="1023" width="11.52" style="8"/>
     <col min="1024" max="1025" width="11.52" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11" t="s">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="13" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1565,33 +1568,33 @@
       <c r="A2" s="6">
         <v>44</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="13"/>
+      <c r="C2" s="12"/>
       <c r="D2" s="6"/>
-      <c r="E2" s="13"/>
+      <c r="E2" s="12"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
-      <c r="J2" s="13"/>
+      <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="6">
         <v>7</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="13"/>
+      <c r="C3" s="12"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="11" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1599,7 +1602,7 @@
       <c r="A4" s="6">
         <v>10</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -1615,13 +1618,13 @@
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
-      <c r="J4" s="15"/>
+      <c r="J4" s="14"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="6">
         <v>11</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -1637,13 +1640,13 @@
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
-      <c r="J5" s="16"/>
+      <c r="J5" s="15"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="6">
         <v>31</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1665,13 +1668,13 @@
       <c r="I6" s="6">
         <v>0</v>
       </c>
-      <c r="J6" s="16"/>
+      <c r="J6" s="15"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="6">
         <v>32</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="6" t="s">
@@ -1693,13 +1696,13 @@
       <c r="I7" s="6">
         <v>0</v>
       </c>
-      <c r="J7" s="16"/>
+      <c r="J7" s="15"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="6">
         <v>33</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>25</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -1721,16 +1724,16 @@
       <c r="I8" s="6">
         <v>0</v>
       </c>
-      <c r="J8" s="15"/>
+      <c r="J8" s="14"/>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="6">
         <v>34</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="13"/>
+      <c r="C9" s="12"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -1745,12 +1748,12 @@
       <c r="A10" s="6">
         <v>37</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="13"/>
+      <c r="C10" s="12"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="13"/>
+      <c r="E10" s="12"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
@@ -1760,27 +1763,40 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="9">
+      <c r="A11" s="8">
         <v>38</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
+      <c r="C11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="9">
+      <c r="A12" s="8">
         <v>12</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>32</v>
+      <c r="B12" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>4</v>
@@ -1798,17 +1814,17 @@
         <v>22</v>
       </c>
       <c r="I12" s="6"/>
-      <c r="J12" s="15"/>
+      <c r="J12" s="14"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="9">
+      <c r="A13" s="8">
         <v>13</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>34</v>
+      <c r="B13" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>4</v>
@@ -1817,26 +1833,26 @@
         <v>0</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I13" s="6"/>
-      <c r="J13" s="15"/>
+      <c r="J13" s="14"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="6">
         <v>14</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>38</v>
+      <c r="B14" s="11" t="s">
+        <v>39</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>14</v>
@@ -1848,17 +1864,17 @@
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="15"/>
+      <c r="J14" s="14"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="6">
         <v>15</v>
       </c>
-      <c r="B15" s="12" t="s">
-        <v>40</v>
+      <c r="B15" s="11" t="s">
+        <v>41</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>20</v>
@@ -1875,17 +1891,17 @@
       <c r="I15" s="6">
         <v>0</v>
       </c>
-      <c r="J15" s="16"/>
+      <c r="J15" s="15"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="6">
         <v>16</v>
       </c>
-      <c r="B16" s="12" t="s">
-        <v>42</v>
+      <c r="B16" s="11" t="s">
+        <v>43</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>20</v>
@@ -1902,17 +1918,17 @@
       <c r="I16" s="6">
         <v>0</v>
       </c>
-      <c r="J16" s="16"/>
+      <c r="J16" s="15"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="6">
         <v>17</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>44</v>
+      <c r="B17" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>20</v>
@@ -1930,17 +1946,17 @@
       <c r="I17" s="6">
         <v>0</v>
       </c>
-      <c r="J17" s="15"/>
+      <c r="J17" s="14"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="6">
         <v>29</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>46</v>
+      <c r="B18" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>4</v>
@@ -1954,17 +1970,17 @@
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
-      <c r="J18" s="15"/>
+      <c r="J18" s="14"/>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="6">
         <v>30</v>
       </c>
-      <c r="B19" s="12" t="s">
-        <v>48</v>
+      <c r="B19" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>20</v>
@@ -1982,17 +1998,17 @@
       <c r="I19" s="6">
         <v>0</v>
       </c>
-      <c r="J19" s="15"/>
+      <c r="J19" s="14"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6">
         <v>18</v>
       </c>
-      <c r="B20" s="12" t="s">
-        <v>50</v>
+      <c r="B20" s="11" t="s">
+        <v>51</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>20</v>
@@ -2010,17 +2026,17 @@
       <c r="I20" s="6">
         <v>0</v>
       </c>
-      <c r="J20" s="15"/>
+      <c r="J20" s="14"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6">
         <v>19</v>
       </c>
-      <c r="B21" s="12" t="s">
-        <v>52</v>
+      <c r="B21" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>20</v>
@@ -2038,17 +2054,17 @@
       <c r="I21" s="6">
         <v>0</v>
       </c>
-      <c r="J21" s="15"/>
+      <c r="J21" s="14"/>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="6">
         <v>21</v>
       </c>
-      <c r="B22" s="12" t="s">
-        <v>54</v>
+      <c r="B22" s="11" t="s">
+        <v>55</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>4</v>
@@ -2062,17 +2078,17 @@
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
-      <c r="J22" s="15"/>
+      <c r="J22" s="14"/>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="6">
         <v>22</v>
       </c>
-      <c r="B23" s="12" t="s">
-        <v>56</v>
+      <c r="B23" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>4</v>
@@ -2086,77 +2102,83 @@
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
-      <c r="J23" s="15"/>
+      <c r="J23" s="14"/>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="6">
         <v>25</v>
       </c>
-      <c r="B24" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
+      <c r="B24" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
+      <c r="F24" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
-      <c r="J24" s="15"/>
+      <c r="J24" s="14"/>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="6">
         <v>26</v>
       </c>
-      <c r="B25" s="12" t="s">
-        <v>59</v>
+      <c r="B25" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>61</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
-      <c r="J25" s="15"/>
+      <c r="J25" s="14"/>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="6">
         <v>27</v>
       </c>
-      <c r="B26" s="12" t="s">
-        <v>62</v>
+      <c r="B26" s="11" t="s">
+        <v>64</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>61</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
-      <c r="J26" s="15"/>
+      <c r="J26" s="14"/>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="6">
         <v>28</v>
       </c>
-      <c r="B27" s="12" t="s">
-        <v>64</v>
+      <c r="B27" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>20</v>
@@ -2174,17 +2196,17 @@
       <c r="I27" s="6">
         <v>0</v>
       </c>
-      <c r="J27" s="15"/>
+      <c r="J27" s="14"/>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="6">
         <v>20</v>
       </c>
-      <c r="B28" s="12" t="s">
-        <v>66</v>
+      <c r="B28" s="11" t="s">
+        <v>68</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>20</v>
@@ -2202,39 +2224,39 @@
       <c r="I28" s="6">
         <v>0</v>
       </c>
-      <c r="J28" s="15"/>
+      <c r="J28" s="14"/>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="6">
         <v>39</v>
       </c>
-      <c r="B29" s="12" t="s">
-        <v>68</v>
+      <c r="B29" s="11" t="s">
+        <v>70</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E29" s="13"/>
+      <c r="E29" s="12"/>
       <c r="F29" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
-      <c r="J29" s="13"/>
+      <c r="J29" s="12"/>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="6">
         <v>40</v>
       </c>
-      <c r="B30" s="12" t="s">
-        <v>70</v>
+      <c r="B30" s="11" t="s">
+        <v>72</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>4</v>
@@ -2248,88 +2270,88 @@
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
-      <c r="J30" s="13"/>
+      <c r="J30" s="12"/>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="6">
         <v>41</v>
       </c>
-      <c r="B31" s="12" t="s">
-        <v>72</v>
+      <c r="B31" s="11" t="s">
+        <v>74</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E31" s="13"/>
+      <c r="E31" s="12"/>
       <c r="F31" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
-      <c r="J31" s="13"/>
+      <c r="J31" s="12"/>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="6">
         <v>42</v>
       </c>
-      <c r="B32" s="12" t="s">
-        <v>74</v>
+      <c r="B32" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E32" s="13"/>
+      <c r="E32" s="12"/>
       <c r="F32" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
-      <c r="J32" s="13"/>
+      <c r="J32" s="12"/>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="6">
         <v>43</v>
       </c>
-      <c r="B33" s="12" t="s">
-        <v>76</v>
+      <c r="B33" s="11" t="s">
+        <v>78</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E33" s="13"/>
+      <c r="E33" s="12"/>
       <c r="F33" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
-      <c r="J33" s="13"/>
+      <c r="J33" s="12"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="6">
         <v>45</v>
       </c>
-      <c r="B34" s="12" t="s">
-        <v>78</v>
+      <c r="B34" s="11" t="s">
+        <v>80</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E34" s="9">
+      <c r="E34" s="8">
         <v>0</v>
       </c>
       <c r="F34" s="6" t="s">
@@ -2343,16 +2365,16 @@
       <c r="A35" s="6">
         <v>46</v>
       </c>
-      <c r="B35" s="12" t="s">
-        <v>80</v>
+      <c r="B35" s="11" t="s">
+        <v>82</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E35" s="9">
+      <c r="E35" s="8">
         <v>0</v>
       </c>
       <c r="F35" s="6" t="s">
@@ -2363,14 +2385,14 @@
       <c r="I35" s="6"/>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="9">
+      <c r="A36" s="8">
         <v>2</v>
       </c>
-      <c r="B36" s="12" t="s">
-        <v>82</v>
+      <c r="B36" s="11" t="s">
+        <v>84</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>20</v>
@@ -2388,28 +2410,28 @@
       <c r="I36" s="6">
         <v>0</v>
       </c>
-      <c r="J36" s="15"/>
+      <c r="J36" s="14"/>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="6">
         <v>3</v>
       </c>
-      <c r="B37" s="12" t="s">
-        <v>84</v>
+      <c r="B37" s="11" t="s">
+        <v>86</v>
       </c>
       <c r="D37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
-      <c r="J37" s="16"/>
+      <c r="J37" s="15"/>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="6">
         <v>4</v>
       </c>
-      <c r="B38" s="12" t="s">
-        <v>85</v>
+      <c r="B38" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
@@ -2417,14 +2439,14 @@
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
-      <c r="J38" s="15"/>
+      <c r="J38" s="14"/>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="6">
         <v>5</v>
       </c>
-      <c r="B39" s="12" t="s">
-        <v>86</v>
+      <c r="B39" s="11" t="s">
+        <v>88</v>
       </c>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
@@ -2433,14 +2455,14 @@
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
-      <c r="J39" s="15"/>
+      <c r="J39" s="14"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6">
         <v>6</v>
       </c>
-      <c r="B40" s="12" t="s">
-        <v>87</v>
+      <c r="B40" s="11" t="s">
+        <v>89</v>
       </c>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
@@ -2448,14 +2470,14 @@
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
-      <c r="J40" s="15"/>
+      <c r="J40" s="14"/>
     </row>
     <row r="41" spans="1:10">
-      <c r="A41" s="9">
+      <c r="A41" s="8">
         <v>1</v>
       </c>
-      <c r="B41" s="12" t="s">
-        <v>88</v>
+      <c r="B41" s="11" t="s">
+        <v>90</v>
       </c>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
@@ -2464,14 +2486,14 @@
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
-      <c r="J41" s="15"/>
+      <c r="J41" s="14"/>
     </row>
     <row r="42" spans="1:10">
-      <c r="A42" s="9">
+      <c r="A42" s="8">
         <v>24</v>
       </c>
-      <c r="B42" s="12" t="s">
-        <v>89</v>
+      <c r="B42" s="11" t="s">
+        <v>91</v>
       </c>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
@@ -2480,14 +2502,14 @@
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
       <c r="I42" s="6"/>
-      <c r="J42" s="15"/>
+      <c r="J42" s="14"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="9">
+      <c r="A43" s="8">
         <v>36</v>
       </c>
-      <c r="B43" s="12" t="s">
-        <v>90</v>
+      <c r="B43" s="11" t="s">
+        <v>92</v>
       </c>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
@@ -2496,14 +2518,14 @@
       <c r="G43" s="6"/>
       <c r="H43" s="6"/>
       <c r="I43" s="6"/>
-      <c r="J43" s="15"/>
+      <c r="J43" s="14"/>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="9">
+      <c r="A44" s="8">
         <v>48</v>
       </c>
-      <c r="B44" s="10" t="s">
-        <v>91</v>
+      <c r="B44" s="9" t="s">
+        <v>93</v>
       </c>
       <c r="D44" s="6"/>
       <c r="F44" s="6"/>
@@ -2512,11 +2534,11 @@
       <c r="I44" s="6"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="9">
+      <c r="A45" s="8">
         <v>9</v>
       </c>
-      <c r="B45" s="12" t="s">
-        <v>92</v>
+      <c r="B45" s="11" t="s">
+        <v>94</v>
       </c>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
@@ -2525,14 +2547,14 @@
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
-      <c r="J45" s="15"/>
+      <c r="J45" s="14"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="9">
+      <c r="A46" s="8">
         <v>23</v>
       </c>
-      <c r="B46" s="12" t="s">
-        <v>93</v>
+      <c r="B46" s="11" t="s">
+        <v>95</v>
       </c>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
@@ -2541,14 +2563,14 @@
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
-      <c r="J46" s="15"/>
+      <c r="J46" s="14"/>
     </row>
     <row r="47" spans="1:10">
-      <c r="A47" s="9">
+      <c r="A47" s="8">
         <v>35</v>
       </c>
-      <c r="B47" s="12" t="s">
-        <v>94</v>
+      <c r="B47" s="11" t="s">
+        <v>96</v>
       </c>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
@@ -2557,14 +2579,14 @@
       <c r="G47" s="6"/>
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
-      <c r="J47" s="15"/>
+      <c r="J47" s="14"/>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="9">
+      <c r="A48" s="8">
         <v>47</v>
       </c>
-      <c r="B48" s="10" t="s">
-        <v>95</v>
+      <c r="B48" s="9" t="s">
+        <v>97</v>
       </c>
       <c r="D48" s="6"/>
       <c r="F48" s="6"/>
@@ -2573,11 +2595,11 @@
       <c r="I48" s="6"/>
     </row>
     <row r="49" spans="1:10">
-      <c r="A49" s="9">
+      <c r="A49" s="8">
         <v>8</v>
       </c>
-      <c r="B49" s="12" t="s">
-        <v>96</v>
+      <c r="B49" s="11" t="s">
+        <v>98</v>
       </c>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
@@ -2586,7 +2608,7 @@
       <c r="G49" s="6"/>
       <c r="H49" s="6"/>
       <c r="I49" s="6"/>
-      <c r="J49" s="15"/>
+      <c r="J49" s="14"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J49">
@@ -2596,22 +2618,22 @@
     <extLst/>
   </autoFilter>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2:H12 H14:H49">
-      <formula1>"LOW,MEDIUM,HIGH,VERY-HIGH"</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F49">
+      <formula1>"NO-PULL,PULL-UP,PULL-DOWN"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D49">
       <formula1>"INPUT,OUTPUT,AF,ANALOG,NA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F49">
-      <formula1>"NO-PULL,PULL-UP,PULL-DOWN"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G13:H13 G2:G12 G14:G49">
       <formula1>"PP,OD"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2:H12 H14:H49">
+      <formula1>"LOW,MEDIUM,HIGH,VERY-HIGH"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="A1 E1:I1 B36 E36 J38 B49 E49 B2:B4 B8:B10 B12:B14 B17:B33 B38:B39 B41:B43 B45:B47 E2:E4 E8:E10 E12:E14 E17:E33 E38:E39 E41:E43 E45:E47 I2:I49"/>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -2621,33 +2643,33 @@
   <sheetPr/>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="20.1133333333333" style="3" customWidth="true"/>
-    <col min="2" max="2" width="19.4866666666667" style="3" customWidth="true"/>
-    <col min="3" max="3" width="10.7266666666667" style="3" customWidth="true"/>
-    <col min="4" max="4" width="11.8533333333333" style="3" customWidth="true"/>
-    <col min="5" max="5" width="63.42" style="3" customWidth="true"/>
-    <col min="6" max="1020" width="8.67333333333333" style="3" customWidth="true"/>
+    <col min="1" max="1" width="20.1133333333333" style="3" customWidth="1"/>
+    <col min="2" max="2" width="19.4866666666667" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.7266666666667" style="3" customWidth="1"/>
+    <col min="4" max="4" width="11.8533333333333" style="3" customWidth="1"/>
+    <col min="5" max="5" width="63.42" style="3" customWidth="1"/>
+    <col min="6" max="1020" width="8.67333333333333" style="3" customWidth="1"/>
     <col min="1021" max="1025" width="11.52" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>9</v>
@@ -2655,13 +2677,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D2" s="3">
         <v>0</v>
@@ -2669,13 +2691,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>104</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>102</v>
       </c>
       <c r="D3" s="5">
         <v>1000</v>
@@ -2683,13 +2705,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D4" s="5">
         <v>0</v>
@@ -2697,13 +2719,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>75</v>
+        <v>109</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>77</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D5" s="5">
         <v>0</v>
@@ -2711,13 +2733,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>112</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D6" s="5">
         <v>1000</v>
@@ -2725,13 +2747,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>114</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D7" s="5">
         <v>0</v>
@@ -2739,47 +2761,47 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D8" s="5">
         <v>0</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="5" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D9" s="5">
         <v>0</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D10" s="5">
         <v>0</v>
@@ -2787,47 +2809,47 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>73</v>
+        <v>119</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D11" s="5">
         <v>0</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="3" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D12" s="5">
         <v>0</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="5" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D13" s="5">
         <v>0</v>
@@ -2835,47 +2857,47 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D14" s="5">
         <v>0</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D15" s="5">
         <v>0</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D16" s="5">
         <v>0</v>
@@ -2883,13 +2905,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="5" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D17" s="5">
         <v>1000</v>
@@ -2897,30 +2919,30 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="5" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D18" s="5">
         <v>29000</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D19" s="5">
         <v>30000</v>
@@ -2934,7 +2956,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2953,31 +2975,31 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelRow="6" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.7733333333333" customWidth="true"/>
-    <col min="2" max="3" width="8.67333333333333" customWidth="true"/>
-    <col min="4" max="5" width="12.5" customWidth="true"/>
-    <col min="6" max="1023" width="8.67333333333333" customWidth="true"/>
+    <col min="1" max="1" width="14.7733333333333" customWidth="1"/>
+    <col min="2" max="3" width="8.67333333333333" customWidth="1"/>
+    <col min="4" max="5" width="12.5" customWidth="1"/>
+    <col min="6" max="1023" width="8.67333333333333" customWidth="1"/>
     <col min="1024" max="1025" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -3119,7 +3141,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>